<commit_message>
[main] Arrange folder and improve occupancy time of PSM.
</commit_message>
<xml_diff>
--- a/Document/Resources.xlsx
+++ b/Document/Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_HKF\_dev\Repository\GSL\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192E921C-F62E-42E2-9930-D0BDA9B49136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A076B5A-1464-4711-943A-C38DB83E81D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{2B8BF1E6-E496-4F89-BDC8-54DCCB78AA27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B8BF1E6-E496-4F89-BDC8-54DCCB78AA27}"/>
   </bookViews>
   <sheets>
     <sheet name="FolderStructure" sheetId="1" r:id="rId1"/>
@@ -1204,28 +1204,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>gsl_xsm.h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> provides XSM shared data types among XSM modules.</t>
-    </r>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>gsl_dsm.h</t>
     </r>
     <r>
@@ -1329,6 +1307,28 @@
   </si>
   <si>
     <t>vidPsmKeepAlive</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>gsl_xsm.h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> provides XSM shared data types among GSL modules.</t>
+    </r>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -6055,8 +6055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33BFA01-738B-4C3B-AB43-466CFAB6F254}">
   <dimension ref="B2:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
@@ -6503,7 +6503,7 @@
       </c>
       <c r="G34" s="105"/>
       <c r="H34" s="111" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.4">
@@ -6516,7 +6516,7 @@
       </c>
       <c r="G35" s="105"/>
       <c r="H35" s="111" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.4">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="G36" s="105"/>
       <c r="H36" s="111" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.4">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="G37" s="105"/>
       <c r="H37" s="111" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.4">
@@ -6568,7 +6568,7 @@
       </c>
       <c r="G39" s="105"/>
       <c r="H39" s="111" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.4">
@@ -6594,7 +6594,7 @@
       </c>
       <c r="G41" s="105"/>
       <c r="H41" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.4">
@@ -7022,7 +7022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202F9C68-BA9B-415A-B4F6-E6F10680B109}">
   <dimension ref="B2:AL112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A58" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
       <selection activeCell="N78" sqref="N78"/>
     </sheetView>
   </sheetViews>
@@ -8283,7 +8283,7 @@
       <c r="K77" s="54"/>
       <c r="L77" s="55"/>
       <c r="N77" s="42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U77" s="81"/>
       <c r="Z77" s="53"/>

</xml_diff>